<commit_message>
make images a little clearer
</commit_message>
<xml_diff>
--- a/analysis/runsByInning/runsByInning.xlsx
+++ b/analysis/runsByInning/runsByInning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\baseballstats\analysis\runsByInning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D1A34-34CF-4861-AE55-9127D3D718EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEFCE93-3DC7-40B7-96D1-CCAFA85EC5EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1823" yWindow="2205" windowWidth="19845" windowHeight="10793" xr2:uid="{A1C1A8EF-FE2F-437D-8A4B-C0A79CF31965}"/>
   </bookViews>
@@ -405,6 +405,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>inning</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -753,6 +808,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>inning</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3450,8 +3560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AAC57D-A1AA-48E1-8BCD-AEA5D5D71549}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
add some spreadsheet data
</commit_message>
<xml_diff>
--- a/analysis/runsByInning/runsByInning.xlsx
+++ b/analysis/runsByInning/runsByInning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\baseballstats\analysis\runsByInning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEFCE93-3DC7-40B7-96D1-CCAFA85EC5EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68AED8D-13CA-40E5-B2E3-84D4138578A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1823" yWindow="2205" windowWidth="19845" windowHeight="10793" xr2:uid="{A1C1A8EF-FE2F-437D-8A4B-C0A79CF31965}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Expected runs</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>(average)</t>
+  </si>
+  <si>
+    <t>average (2-8 innings)</t>
+  </si>
+  <si>
+    <t>visitor runs</t>
+  </si>
+  <si>
+    <t>"expected" runs in bottom 1st</t>
   </si>
 </sst>
 </file>
@@ -3558,10 +3567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AAC57D-A1AA-48E1-8BCD-AEA5D5D71549}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4138,6 +4147,85 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4.088664000000003E-2</v>
+      </c>
+      <c r="D20">
+        <v>5.1468940000000019E-2</v>
+      </c>
+      <c r="E20">
+        <v>3.7220049999999949E-2</v>
+      </c>
+      <c r="F20">
+        <v>5.0651180000000073E-2</v>
+      </c>
+      <c r="G20">
+        <v>3.8051040000000036E-2</v>
+      </c>
+      <c r="H20">
+        <v>3.7499179999999965E-2</v>
+      </c>
+      <c r="I20">
+        <v>2.8128180000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGE(C20:I20)</f>
+        <v>4.0557887142857151E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.42001822999999999</v>
+      </c>
+      <c r="D22">
+        <v>0.47471341</v>
+      </c>
+      <c r="E22">
+        <v>0.48881805</v>
+      </c>
+      <c r="F22">
+        <v>0.47699841999999998</v>
+      </c>
+      <c r="G22">
+        <v>0.49805546000000001</v>
+      </c>
+      <c r="H22">
+        <v>0.47474771999999998</v>
+      </c>
+      <c r="I22">
+        <v>0.4656074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(C22:I22)</f>
+        <v>0.47127981285714288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <f>B2*(1+C21/C23)</f>
+        <v>0.5493613516037662</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>